<commit_message>
Changed the Art to an art gallery
Instead of links, artwork can now be viewed as a gallery
</commit_message>
<xml_diff>
--- a/data/geography_data.xlsx
+++ b/data/geography_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\anp-website\alexandpedro.github.io\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9FF1FD5-4760-43D7-9A8E-53F5E5904741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9564B3-0303-4DD6-9BDE-9653AF94DB31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3210" yWindow="690" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="geography_data" sheetId="1" r:id="rId1"/>
@@ -2258,9 +2258,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S211"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F76" sqref="F76"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D155" sqref="D155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>